<commit_message>
Fixing failures - BCT
</commit_message>
<xml_diff>
--- a/resources/testdata/UserSearchTestCase.xlsx
+++ b/resources/testdata/UserSearchTestCase.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
-    <sheet name="searchLoginName" sheetId="2" r:id="rId2"/>
-    <sheet name="searchFirstName" sheetId="3" r:id="rId3"/>
-    <sheet name="searchLastName" sheetId="4" r:id="rId4"/>
-    <sheet name="searchEmail" sheetId="5" r:id="rId5"/>
-    <sheet name="searchAll" sheetId="6" r:id="rId6"/>
-    <sheet name="testResetWithAllData" sheetId="7" r:id="rId7"/>
+    <sheet name="lookforUser" sheetId="8" r:id="rId2"/>
+    <sheet name="searchLoginName" sheetId="2" r:id="rId3"/>
+    <sheet name="searchFirstName" sheetId="3" r:id="rId4"/>
+    <sheet name="searchLastName" sheetId="4" r:id="rId5"/>
+    <sheet name="searchEmail" sheetId="5" r:id="rId6"/>
+    <sheet name="searchAll" sheetId="6" r:id="rId7"/>
+    <sheet name="testResetWithAllData" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="27">
   <si>
     <t>TCID</t>
   </si>
@@ -95,6 +96,12 @@
   </si>
   <si>
     <t>Deactivate</t>
+  </si>
+  <si>
+    <t>shortLoginName</t>
+  </si>
+  <si>
+    <t>autotestuser1</t>
   </si>
 </sst>
 </file>
@@ -446,7 +453,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +540,68 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +615,7 @@
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -569,8 +637,11 @@
       <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -591,6 +662,9 @@
       </c>
       <c r="G2" t="s">
         <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -659,7 +733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -720,7 +794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -781,7 +855,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -840,65 +985,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>